<commit_message>
changes added to tracker
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shesh\Desktop\sheshank_doc\ML\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198DB350-EC84-4E41-873A-F2694AD914EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72ECF84-1E2D-43A3-B593-41697C01BC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="645" firstSheet="3" activeTab="11" xr2:uid="{D7F2B556-C617-4DDF-8866-32B87C862FE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="645" firstSheet="4" activeTab="4" xr2:uid="{D7F2B556-C617-4DDF-8866-32B87C862FE3}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="ADA BOOST" sheetId="15" r:id="rId21"/>
     <sheet name="CAT BOOST" sheetId="16" r:id="rId22"/>
     <sheet name="LGB" sheetId="17" r:id="rId23"/>
+    <sheet name="kmeans" sheetId="26" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="1208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="1211">
   <si>
     <t>Topic</t>
   </si>
@@ -9594,117 +9595,6 @@
 which was provided by the training data and when new data is given as input to the model if same kind of feature values arise the outcome will be same</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Linearity:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> The relationship between the independent variables and the dependent variable should be linear. This means that a change in the independent variable(s) should result in a proportional change in the dependent variable. You can check this assumption by examining scatterplots and residual plots.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Normality of Errors:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> The errors should be normally distributed. This assumption is not about the normality of the independent variables but the normality of the residuals. Normality ensures that the parameter estimates are efficient and unbiased. You can check this assumption using techniques like a normal probability plot or a histogram of residuals.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>No or Little Multicollinearity</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: If you have multiple independent variables in your model, they should not be highly correlated with each other. High multicollinearity can make it difficult to determine the individual effect of each predictor on the dependent variable.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Homoscedasticity (Constant Variance of Errors):</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> The variance of the errors should be constant across all levels of the independent variables. In simpler terms, the spread of residuals should be roughly consistent throughout the range of the predictor variables. Heteroscedasticity, where the variance changes systematically, can be a violation of this assumption.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Independence of Errors:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> The errors (residuals) should be independent of each other. In other words, the error for one observation should not be correlated with the errors for other observations. Autocorrelation or serial correlation can violate this assumption.</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">What are the various metrcs to consider in order to assess the performance of the linear regression model? </t>
   </si>
   <si>
@@ -18797,6 +18687,176 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>methods to check normality assumption?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Shapiro-Wilk Test:
+Method: Perform the Shapiro-Wilk test, a statistical test for normality. The null hypothesis is that the data is normally distributed.
+Interpretation: If the p-value is greater than the chosen significance level (e.g., 0.05), you fail to reject the null hypothesis, suggesting normality.
+4. Kolmogorov-Smirnov Test:
+Method: Similar to the Shapiro-Wilk test, the Kolmogorov-Smirnov test assesses whether the sample distribution is significantly different from a normal distribution.
+Interpretation: A higher p-value indicates that the data is consistent with normality.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Durbin-Watson Test:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Method: A statistical test that assesses autocorrelation by examining the correlation between consecutive residuals.
+Interpretation: The test statistic ranges from 0 to 4, with values close to 2 indicating no autocorrelation. Values significantly below 2 (less than 1.5) suggest positive autocorrelation, while values significantly above 2 (greater than 2.5) suggest negative autocorrelation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Linearity:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The relationship between the independent variables and the dependent variable should be linear. This means that a change in the independent variable(s) should result in a proportional change in the dependent variable. You can check this assumption by examining scatterplots and residual plots. If this assumption is violated, the model may fail to accurately capture the underlying pattern in the data.
+If the linearity assumption is violated, one might consider using polynomial regression or transforming the variables to better capture the non-linear relationship.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Normality of Errors:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The errors should be normally distributed. This assumption is not about the normality of the independent variables but the normality of the residuals. You can check this assumption using techniques like a normal probability plot or a histogram of residuals.
+The assumption of normality of residuals in linear regression is not critical for large sample sizes, thanks to the Central Limit Theorem. However, for smaller sample sizes, departures from normality can impact the reliability of statistical tests associated with the regression coefficients and can affect the accuracy of confidence intervals.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No or Little Multicollinearity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: If you have multiple independent variables in your model, they should not be highly correlated with each other. High multicollinearity can make it difficult to determine the individual effect of each predictor on the dependent variable.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Homoscedasticity (Constant Variance of Errors):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The variance of the errors should be constant across all levels of the independent variables. In simpler terms, the spread of residuals should be roughly consistent throughout the range of the predictor variables. Heteroscedasticity, where the variance changes systematically, can be a violation of this assumption.
+This means that the estimates may have larger standard errors, reducing the precision of the estimates. As a result, confidence intervals for the coefficients may be wider.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Independence of Errors:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The errors (residuals) should be independent of each other. In other words, the error for one observation should not be correlated with the errors for other observations. Autocorrelation or serial correlation can violate this assumption.
+Autocorrelation often indicates the presence of a systematic pattern or structure in the residuals over time. This suggests that the model is not adequately capturing the temporal dynamics of the data, and predictions may be influenced by past errors.
+Standard hypothesis tests, such as t-tests and F-tests, rely on the assumption of independent and identically distributed residuals. If this assumption is violated, the p-values associated with these tests may be unreliable, leading to incorrect conclusions about the significance of the regression coefficients or the overall model.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Linearity:
 </t>
     </r>
@@ -18839,6 +18899,7 @@
 A random scatter of residuals around the horizontal axis suggests constant variance. If the spread of residuals is relatively consistent as the predicted values increase, homoscedasticity is likely satisfied. Ensure a consistent spread of points; avoid patterns like a funnel shape.
 Homoscedasticity is violated if the spread does not remain consistent across the range of fitted values.
 If the spread of residuals systematically changes with different levels of predictors, homoscedasticity is not met.
+A funnel-like shape in a residual plot typically indicates the presence of heteroscedasticity, which means that the variance of the residuals is not constant across all levels of the independent variable(s).
 what happens if the model doesn't follow homoscedasticity?
 When a linear regression model violates the assumption of homoscedasticity (constant variance of residuals), it can lead to inefficient parameter estimates and biased standard errors.
 Apply a transformation to the dependent variable, such as taking the logarithm.
@@ -18867,7 +18928,7 @@
       <t xml:space="preserve">
 Plot the residuals against the fitted (predicted) values.
 Look for a random scatter of points with no discernible pattern. If there is a pattern, it may suggest a violation of independence.
-Include lagged values of the residuals as additional predictors in the model if the model suffers with autocorrelation. Assign weights to observations based on the degree of autocorrelation.
+Include lagged values of the residuals as additional predictors in the model if the model suffers with autocorrelation. Assign weights to observations based on the degree of autocorrelation.  If autocorrelation is present, you might observe a pattern where residuals are not randomly scattered but show some form of structure.
 If there is Auto correlation within the data and the dataset belong to time series then make use of time series models like ARIMA.
  </t>
     </r>
@@ -18882,48 +18943,340 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>methods to check normality assumption?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Shapiro-Wilk Test:
-Method: Perform the Shapiro-Wilk test, a statistical test for normality. The null hypothesis is that the data is normally distributed.
-Interpretation: If the p-value is greater than the chosen significance level (e.g., 0.05), you fail to reject the null hypothesis, suggesting normality.
-4. Kolmogorov-Smirnov Test:
-Method: Similar to the Shapiro-Wilk test, the Kolmogorov-Smirnov test assesses whether the sample distribution is significantly different from a normal distribution.
-Interpretation: A higher p-value indicates that the data is consistent with normality.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Durbin-Watson Test:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Method: A statistical test that assesses autocorrelation by examining the correlation between consecutive residuals.
-Interpretation: The test statistic ranges from 0 to 4, with values close to 2 indicating no autocorrelation. Values significantly below 2 (less than 1.5) suggest positive autocorrelation, while values significantly above 2 (greater than 2.5) suggest negative autocorrelation.</t>
+      <t>Data Cleaning:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Remove or handle missing values in the dataset.
+Check for outliers and decide whether to remove or transform them based on the nature of your data.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Feature Scaling:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Normalize or standardize the features to ensure that all variables contribute equally to the distance computations. Common scaling methods include Min-Max scaling or Z-score normalization.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Handling Categorical Variables:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">If your dataset contains categorical variables, convert them into a numerical format. This may involve one-hot encoding, label encoding, or other techniques depending on the nature of the categorical variables.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Feature Selection:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Assess whether all features are relevant for clustering. Remove irrelevant or redundant features to simplify the model and potentially improve the clustering results.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Remove Duplicates:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Check for and remove any duplicate rows in the dataset.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Handling High-Dimensional Data:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If the dataset has a high number of dimensions (features), consider dimensionality reduction techniques such as Principal Component Analysis (PCA) to reduce the number of features while preserving the most important information.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Understanding Domain Knowledge:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Gain insights into the domain of your data to inform decisions about the number of clusters (K) and the interpretability of the results. Understanding the nature of the data can help in choosing an appropriate distance metric and initializations.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Choosing the Right Distance Metric:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Depending on the nature of your data, choose an appropriate distance metric (e.g., Euclidean distance, Manhattan distance, cosine similarity) that aligns with the characteristics of your features.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Determining the Number of Clusters (K):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Decide on the appropriate number of clusters for your specific problem. You can use techniques such as the elbow method, silhouette analysis, or domain knowledge to help determine the optimal number of clusters.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Initial Centroid Placement:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Consider using smart initialization techniques, such as K-means++, to improve the convergence speed and the quality of the final clusters.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>How to decide when to use which technique to detect outliers?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Z-Score Method:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> It assumes that the data follows a normal distribution.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IQR (Interquartile Range) Method:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  It is robust to outliers and works well for skewed distributions. Use this method when your data is skewed or not normally distributed.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DBSCAN: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Use this method when your data has clusters or density variations.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Isolation Forest:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  It is effective for high-dimensional data and can handle mixed data types. Use this method for datasets with mixed data types or high dimensionality.
+</t>
     </r>
   </si>
 </sst>
@@ -19364,7 +19717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -19530,12 +19883,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -20237,37 +20584,37 @@
   <sheetData>
     <row r="1" spans="2:2" ht="72" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="2" spans="2:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="345.6" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
   </sheetData>
@@ -20291,98 +20638,98 @@
   <sheetData>
     <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="163.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>1116</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1117</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="166.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="319.2" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
   </sheetData>
@@ -20394,8 +20741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B5D22B-731D-4B12-B5EB-ED12599E6F65}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20428,38 +20775,38 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="403.2" x14ac:dyDescent="0.3">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1205</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -20486,13 +20833,13 @@
     </row>
     <row r="12" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
+        <v>824</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>825</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>798</v>
       </c>
@@ -20587,7 +20934,7 @@
         <v>140</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>141</v>
@@ -20598,7 +20945,7 @@
         <v>810</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C28" s="11"/>
     </row>
@@ -20607,7 +20954,7 @@
         <v>142</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="271.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -20655,7 +21002,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>137</v>
       </c>
@@ -20691,7 +21038,7 @@
         <v>143</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
@@ -20713,7 +21060,7 @@
         <v>144</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="331.2" x14ac:dyDescent="0.3">
@@ -20777,15 +21124,15 @@
         <v>147</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1014</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1015</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
@@ -20793,7 +21140,7 @@
         <v>151</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
@@ -20801,7 +21148,7 @@
         <v>152</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -20814,17 +21161,17 @@
     </row>
     <row r="7" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
@@ -20941,18 +21288,18 @@
     </row>
     <row r="3" spans="1:2" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
@@ -21094,7 +21441,7 @@
         <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -21140,7 +21487,7 @@
         <v>201</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -21174,7 +21521,7 @@
         <v>208</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
   </sheetData>
@@ -21332,7 +21679,7 @@
         <v>238</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -21368,7 +21715,7 @@
         <v>240</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -21408,10 +21755,10 @@
     </row>
     <row r="14" spans="1:3" ht="267" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>1146</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>1147</v>
       </c>
       <c r="C14" s="11"/>
     </row>
@@ -21420,7 +21767,7 @@
         <v>241</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -21430,10 +21777,10 @@
     </row>
     <row r="17" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>1149</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>1150</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -21554,12 +21901,12 @@
         <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -21567,7 +21914,7 @@
         <v>244</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -21583,7 +21930,7 @@
         <v>287</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -21596,10 +21943,10 @@
     </row>
     <row r="8" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="345" x14ac:dyDescent="0.35">
@@ -21607,7 +21954,7 @@
         <v>817</v>
       </c>
       <c r="B9" s="54" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -21620,78 +21967,78 @@
     </row>
     <row r="11" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>839</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>844</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -21705,7 +22052,7 @@
     <row r="24" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -21772,20 +22119,20 @@
         <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -21801,32 +22148,32 @@
         <v>320</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -21849,22 +22196,22 @@
     </row>
     <row r="15" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="144" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="144" x14ac:dyDescent="0.3">
@@ -21907,96 +22254,96 @@
     </row>
     <row r="2" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="B15" s="52" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
   </sheetData>
@@ -22040,7 +22387,7 @@
     </row>
     <row r="3" spans="1:3" ht="186" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="C3" s="11"/>
     </row>
@@ -22058,15 +22405,15 @@
         <v>320</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
@@ -22076,12 +22423,12 @@
     </row>
     <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -22110,7 +22457,7 @@
     </row>
     <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -22237,7 +22584,7 @@
         <v>401</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -22272,20 +22619,20 @@
         <v>337</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="252" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="292.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -22298,18 +22645,18 @@
     </row>
     <row r="15" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>1161</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1162</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -22347,17 +22694,17 @@
     </row>
     <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
   </sheetData>
@@ -22396,12 +22743,12 @@
         <v>167</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -22422,7 +22769,7 @@
     </row>
     <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
@@ -22443,17 +22790,17 @@
     </row>
     <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -22513,12 +22860,40 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5242491-7AEE-4FAF-BB3C-97EDEE98475C}">
+  <dimension ref="B1:B2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="101.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DFB714-F672-402F-8602-5E61FD901C54}">
   <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22546,13 +22921,13 @@
     <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -22572,7 +22947,7 @@
         <v>269</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="360" x14ac:dyDescent="0.3">
@@ -22580,7 +22955,7 @@
         <v>270</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -22588,7 +22963,7 @@
         <v>272</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -22596,7 +22971,7 @@
         <v>562</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
@@ -22604,19 +22979,19 @@
         <v>563</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -22662,12 +23037,12 @@
         <v>573</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="159" thickBot="1" x14ac:dyDescent="0.35">
@@ -22675,7 +23050,7 @@
         <v>564</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
@@ -22683,15 +23058,15 @@
         <v>574</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>1133</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>1134</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="354.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -22699,15 +23074,15 @@
         <v>575</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -22738,10 +23113,10 @@
     </row>
     <row r="30" spans="1:2" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -22749,7 +23124,7 @@
         <v>580</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -22757,23 +23132,23 @@
         <v>261</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>941</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>942</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>970</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.35">
@@ -22781,7 +23156,7 @@
         <v>581</v>
       </c>
       <c r="B35" s="38" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -22797,7 +23172,7 @@
         <v>584</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -22836,7 +23211,7 @@
         <v>592</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.35">
@@ -22847,12 +23222,12 @@
         <v>596</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" ht="121.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>597</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="90" x14ac:dyDescent="0.35">
@@ -22873,10 +23248,10 @@
     </row>
     <row r="48" spans="1:2" ht="405" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
+        <v>945</v>
+      </c>
+      <c r="B48" s="36" t="s">
         <v>946</v>
-      </c>
-      <c r="B48" s="36" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -22884,7 +23259,7 @@
         <v>594</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -22892,7 +23267,7 @@
         <v>595</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
@@ -22908,7 +23283,7 @@
     </row>
     <row r="53" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -22916,7 +23291,7 @@
         <v>602</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
@@ -22926,7 +23301,7 @@
     </row>
     <row r="56" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -22977,7 +23352,7 @@
         <v>604</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -22990,10 +23365,10 @@
     </row>
     <row r="67" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -23006,12 +23381,12 @@
     </row>
     <row r="69" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="B70" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -23024,10 +23399,10 @@
     </row>
     <row r="72" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>975</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.35">
@@ -23035,7 +23410,7 @@
         <v>690</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="30" x14ac:dyDescent="0.3">
@@ -23050,10 +23425,10 @@
     </row>
     <row r="76" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -23063,7 +23438,7 @@
     </row>
     <row r="78" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
   </sheetData>
@@ -23102,12 +23477,12 @@
     </row>
     <row r="4" spans="1:4" ht="345.6" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
@@ -23115,7 +23490,7 @@
         <v>520</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="216" x14ac:dyDescent="0.3">
@@ -23183,7 +23558,7 @@
     <row r="16" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="8" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="403.2" x14ac:dyDescent="0.3">
@@ -23229,7 +23604,7 @@
         <v>557</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="141" customHeight="1" x14ac:dyDescent="0.3">
@@ -23253,7 +23628,7 @@
         <v>631</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="295.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -23266,19 +23641,19 @@
     </row>
     <row r="26" spans="1:4" ht="274.8" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="210" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
@@ -23292,15 +23667,15 @@
     <row r="30" spans="1:4" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A30" s="32"/>
       <c r="B30" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A31" s="32" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="200.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -23308,7 +23683,7 @@
         <v>607</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="144" x14ac:dyDescent="0.3">
@@ -23326,10 +23701,10 @@
     </row>
     <row r="35" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
+        <v>830</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>831</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="300" x14ac:dyDescent="0.35">
@@ -23337,7 +23712,7 @@
         <v>491</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="72" x14ac:dyDescent="0.3">
@@ -23355,7 +23730,7 @@
         <v>615</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
@@ -23384,7 +23759,7 @@
         <v>617</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -23392,7 +23767,7 @@
         <v>618</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="144" x14ac:dyDescent="0.3">
@@ -23432,7 +23807,7 @@
         <v>13</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
@@ -23456,7 +23831,7 @@
         <v>16</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
@@ -23469,10 +23844,10 @@
     </row>
     <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>1039</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>1040</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
@@ -23480,7 +23855,7 @@
         <v>624</v>
       </c>
       <c r="B53" s="55" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
@@ -23496,21 +23871,21 @@
         <v>261</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>1043</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>1044</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="360" x14ac:dyDescent="0.3">
@@ -23518,7 +23893,7 @@
         <v>7</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -23617,7 +23992,7 @@
         <v>72</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -23627,7 +24002,7 @@
         <v>75</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -23657,17 +24032,17 @@
         <v>80</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="75" t="s">
-        <v>1202</v>
+      <c r="A73" s="14" t="s">
+        <v>1201</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -23691,13 +24066,13 @@
         <v>215</v>
       </c>
       <c r="B76" s="36" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="60" x14ac:dyDescent="0.35">
       <c r="A77" s="6"/>
       <c r="B77" s="36" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -23748,7 +24123,7 @@
         <v>210</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
@@ -23800,15 +24175,15 @@
         <v>643</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A90" s="14" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>1049</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -24073,10 +24448,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F9766C-5467-4C6A-856C-E91C39450D47}">
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24115,7 +24490,7 @@
     <row r="4" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
       <c r="B4" s="21" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
@@ -24182,7 +24557,7 @@
         <v>166</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -24193,22 +24568,22 @@
     </row>
     <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
-      <c r="B14" s="74" t="s">
-        <v>1195</v>
+      <c r="B14" s="1" t="s">
+        <v>1194</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
       <c r="B15" s="1" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
@@ -24252,7 +24627,7 @@
     <row r="21" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -24270,7 +24645,7 @@
     <row r="23" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -24308,7 +24683,7 @@
     <row r="27" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="3" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -24318,17 +24693,17 @@
         <v>7</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -24415,20 +24790,20 @@
     </row>
     <row r="38" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>1142</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>1143</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>1144</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>1145</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -24438,7 +24813,7 @@
         <v>55</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -24479,10 +24854,10 @@
     </row>
     <row r="45" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>1185</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>1186</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -24490,7 +24865,7 @@
         <v>56</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>58</v>
@@ -24500,7 +24875,7 @@
     <row r="47" spans="1:4" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -24523,43 +24898,43 @@
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="111.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="3" t="s">
-        <v>1188</v>
+        <v>1210</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+    <row r="51" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="5"/>
+      <c r="B51" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>1189</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="B52" s="3" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="5"/>
-      <c r="B52" s="3" t="s">
-        <v>1190</v>
-      </c>
-      <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" ht="282.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="3" t="s">
-        <v>1192</v>
+        <v>1189</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:4" ht="189" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="282.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="3" t="s">
         <v>1191</v>
@@ -24567,588 +24942,596 @@
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="189" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="3" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="3" t="s">
-        <v>69</v>
+        <v>1192</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
-        <v>487</v>
-      </c>
+    <row r="57" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="5"/>
       <c r="B57" s="3" t="s">
-        <v>489</v>
+        <v>69</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>61</v>
+        <v>487</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A59" s="71" t="s">
+    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A60" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="10">
+      <c r="C60" s="2"/>
+      <c r="D60" s="10">
         <v>44935</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A60" s="71"/>
-      <c r="B60" s="3" t="s">
-        <v>833</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A61" s="71"/>
       <c r="B61" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A62" s="71"/>
+      <c r="B62" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A62" s="42" t="s">
-        <v>834</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>835</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="5"/>
+    <row r="63" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A63" s="42" t="s">
+        <v>833</v>
+      </c>
       <c r="B63" s="3" t="s">
-        <v>86</v>
+        <v>834</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="3" t="s">
-        <v>484</v>
+        <v>86</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="8" t="s">
-        <v>91</v>
-      </c>
+    <row r="65" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="5"/>
       <c r="B65" s="3" t="s">
-        <v>92</v>
+        <v>484</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="5" t="s">
-        <v>88</v>
+    <row r="66" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="71" t="s">
-        <v>117</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>118</v>
-      </c>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A70" s="71"/>
+    <row r="70" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="71" t="s">
+        <v>117</v>
+      </c>
       <c r="B70" s="3" t="s">
-        <v>1135</v>
+        <v>118</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A71" s="71"/>
       <c r="B71" s="3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" ht="403.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="71"/>
+      <c r="B72" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C71" s="12" t="s">
+      <c r="C72" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="42"/>
-      <c r="B72" s="3" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C72" s="12"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A73" s="42"/>
       <c r="B73" s="3" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="C73" s="12"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
+    <row r="74" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A74" s="42"/>
+      <c r="B74" s="3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C74" s="12"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" ht="201" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" ht="201" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A78" s="6"/>
-      <c r="B78" s="1" t="s">
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A79" s="6"/>
+      <c r="B79" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="6" t="s">
+    <row r="80" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A80" s="6"/>
-      <c r="B80" s="1" t="s">
+    <row r="81" spans="1:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A81" s="6"/>
+      <c r="B81" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A81" s="71" t="s">
+    <row r="82" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A82" s="71" t="s">
         <v>229</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B82" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
-      <c r="A82" s="71"/>
-      <c r="B82" s="3" t="s">
+    <row r="83" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A83" s="71"/>
+      <c r="B83" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A83" s="6" t="s">
+    <row r="84" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A84" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="6" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A85" s="6"/>
-      <c r="B85" s="1" t="s">
+    <row r="86" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A86" s="6"/>
+      <c r="B86" s="1" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A86" s="6" t="s">
+    <row r="87" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A87" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A87" s="15" t="s">
+    <row r="88" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A88" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="C88" s="11" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="4" t="s">
+    <row r="89" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="4" t="s">
+    <row r="90" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="288" x14ac:dyDescent="0.3">
-      <c r="A90" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="288" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="288" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C92" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A92" s="4" t="s">
+    <row r="93" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A93" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="4" t="s">
+    <row r="94" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C94" s="11" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A94" s="16" t="s">
+    <row r="95" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A95" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C94" s="11"/>
-    </row>
-    <row r="96" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A96" s="4" t="s">
+      <c r="C95" s="11"/>
+    </row>
+    <row r="97" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C97" s="11" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="s">
+    <row r="98" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A98" s="4" t="s">
+    <row r="99" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A99" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="A99" s="4" t="s">
+    <row r="100" spans="1:3" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A100" s="4" t="s">
+    <row r="101" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A101" s="4" t="s">
+    <row r="102" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B102" s="1"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B103" s="1"/>
     </row>
-    <row r="104" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B104" s="1"/>
+    </row>
+    <row r="105" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C105" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
+    <row r="106" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="C105" s="11" t="s">
+      <c r="C106" s="11" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
+    <row r="107" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B107" s="1" t="s">
+    <row r="108" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B108" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="4" t="s">
+    <row r="109" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="216" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="s">
+    <row r="110" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+      <c r="A110" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C110" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" s="4" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
-      <c r="A113" s="4" t="s">
+    <row r="114" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A114" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="B113" s="28" t="s">
+      <c r="B114" s="28" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A114" s="4" t="s">
+    <row r="115" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A115" s="69" t="s">
+    <row r="116" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A116" s="69" t="s">
         <v>378</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B116" s="1" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="288" x14ac:dyDescent="0.3">
-      <c r="A116" s="69"/>
-      <c r="B116" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C116" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" ht="288" x14ac:dyDescent="0.3">
       <c r="A117" s="69"/>
       <c r="B117" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="345.6" x14ac:dyDescent="0.3">
+        <v>381</v>
+      </c>
+      <c r="C117" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A118" s="69"/>
       <c r="B118" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A119" s="69"/>
       <c r="B119" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A120" s="69"/>
+      <c r="B120" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="336" x14ac:dyDescent="0.3">
-      <c r="A120" s="4" t="s">
+    <row r="121" spans="1:3" ht="336" x14ac:dyDescent="0.3">
+      <c r="A121" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C120" s="11" t="s">
+      <c r="C121" s="11" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" s="4" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B122" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A122" s="4" t="s">
+    <row r="123" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A123" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B123" s="1" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" s="4" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="4" t="s">
         <v>693</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A115:A119"/>
+    <mergeCell ref="A116:A120"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A82:A83"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C71" r:id="rId1" display="https://www.youtube.com/watch?v=gzrQvzYEvYc&amp;t=249s" xr:uid="{037A6B83-99E9-4A12-AA81-809B626C745F}"/>
-    <hyperlink ref="C90" r:id="rId2" xr:uid="{3D33C826-7135-4519-B140-F675D1123A86}"/>
-    <hyperlink ref="C91" r:id="rId3" xr:uid="{3824DA84-47CF-4D31-AA0E-04A22DAD8BCE}"/>
-    <hyperlink ref="C93" r:id="rId4" xr:uid="{66F746C5-1015-44FE-BFBA-28D184B276B8}"/>
+    <hyperlink ref="C72" r:id="rId1" display="https://www.youtube.com/watch?v=gzrQvzYEvYc&amp;t=249s" xr:uid="{037A6B83-99E9-4A12-AA81-809B626C745F}"/>
+    <hyperlink ref="C91" r:id="rId2" xr:uid="{3D33C826-7135-4519-B140-F675D1123A86}"/>
+    <hyperlink ref="C92" r:id="rId3" xr:uid="{3824DA84-47CF-4D31-AA0E-04A22DAD8BCE}"/>
+    <hyperlink ref="C94" r:id="rId4" xr:uid="{66F746C5-1015-44FE-BFBA-28D184B276B8}"/>
     <hyperlink ref="C9" r:id="rId5" xr:uid="{4A4AA6B2-6479-419C-A043-9A61CB3C148B}"/>
     <hyperlink ref="C2" r:id="rId6" display="https://mlbookcamp.com/article/crisp-dm" xr:uid="{366E00BF-8318-47E5-8DD6-FE47524E075A}"/>
-    <hyperlink ref="C120" r:id="rId7" xr:uid="{50359122-829B-4B46-A956-184AC67969EC}"/>
-    <hyperlink ref="C105" r:id="rId8" xr:uid="{E5974F08-1C76-43F2-8662-9BFAD160AD79}"/>
+    <hyperlink ref="C121" r:id="rId7" xr:uid="{50359122-829B-4B46-A956-184AC67969EC}"/>
+    <hyperlink ref="C106" r:id="rId8" xr:uid="{E5974F08-1C76-43F2-8662-9BFAD160AD79}"/>
     <hyperlink ref="C31" r:id="rId9" xr:uid="{F7D9DEE8-C3EF-40AC-B83C-C3F5C55EF822}"/>
-    <hyperlink ref="C96" r:id="rId10" xr:uid="{18BEAC28-0E2B-42CA-BDB0-170742EE9127}"/>
-    <hyperlink ref="C87" r:id="rId11" xr:uid="{91679E8C-53A8-4FFC-9692-717359315E93}"/>
+    <hyperlink ref="C97" r:id="rId10" xr:uid="{18BEAC28-0E2B-42CA-BDB0-170742EE9127}"/>
+    <hyperlink ref="C88" r:id="rId11" xr:uid="{91679E8C-53A8-4FFC-9692-717359315E93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
@@ -25206,8 +25589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112F4E25-B6EF-4FC2-AAC0-B362CEC80063}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25250,7 +25633,7 @@
     </row>
     <row r="5" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -25260,7 +25643,7 @@
     </row>
     <row r="7" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -25288,7 +25671,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="288" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>758</v>
       </c>
@@ -25557,7 +25940,7 @@
         <v>57</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -25625,7 +26008,7 @@
     <row r="63" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -25649,7 +26032,7 @@
         <v>543</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -25657,10 +26040,10 @@
         <v>544</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="C67" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
@@ -25713,7 +26096,7 @@
         <v>201</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -25737,7 +26120,7 @@
         <v>208</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
   </sheetData>
@@ -25770,245 +26153,245 @@
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="4" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" s="56" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="60" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B4" s="61" t="s">
         <v>1092</v>
-      </c>
-      <c r="B4" s="61" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="4" customFormat="1" ht="273.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="58" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B5" s="59" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="4" customFormat="1" ht="216" x14ac:dyDescent="0.3">
       <c r="A6" s="69" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="4" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A7" s="69"/>
       <c r="B7" s="1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="44"/>
       <c r="B8" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="66" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="64"/>
       <c r="B9" s="65" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="44"/>
       <c r="B10" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="44"/>
       <c r="B11" s="1" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="4" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="15" spans="1:2" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>1095</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1096</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="4" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="4" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="66" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B19" s="65" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="66" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B20" s="65" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="66" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B21" s="65" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="66" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B22" s="67" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="66" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B23" s="65" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="24" spans="1:2" s="4" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="4" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="26" spans="1:2" s="4" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B26" s="14" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="4" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="31" spans="1:2" s="4" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="4" customFormat="1" ht="317.39999999999998" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="4" customFormat="1" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="47" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="47"/>
       <c r="B34" s="48" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="4" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="49" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B35" s="48" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36" s="72" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="4" customFormat="1" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="73"/>
       <c r="B37" s="45" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="4" customFormat="1" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
+        <v>898</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>899</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="4" customFormat="1" ht="216.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="47" t="s">
+        <v>900</v>
+      </c>
+      <c r="B39" s="50" t="s">
         <v>901</v>
-      </c>
-      <c r="B39" s="50" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="4" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="4" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="42" spans="1:2" s="4" customFormat="1" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
@@ -26016,7 +26399,7 @@
         <v>731</v>
       </c>
       <c r="B42" s="48" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="43" spans="1:2" s="4" customFormat="1" ht="159" thickBot="1" x14ac:dyDescent="0.35">
@@ -26024,54 +26407,54 @@
         <v>4</v>
       </c>
       <c r="B43" s="46" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="44" spans="1:2" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="45" spans="1:2" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
+        <v>910</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>911</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="46" spans="1:2" s="4" customFormat="1" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
+        <v>912</v>
+      </c>
+      <c r="B46" s="51" t="s">
         <v>913</v>
-      </c>
-      <c r="B46" s="51" t="s">
-        <v>914</v>
       </c>
     </row>
     <row r="47" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="48" spans="1:2" s="4" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="49" spans="1:2" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="50" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B50" s="1"/>
     </row>
@@ -26260,12 +26643,12 @@
     </row>
     <row r="2" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -26281,196 +26664,196 @@
         <v>701</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>848</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>849</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="210" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>854</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>855</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
   </sheetData>

</xml_diff>